<commit_message>
19 August 2019 BCP002_Test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ClientData" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="ContactData" sheetId="2" r:id="rId3"/>
     <sheet name="AddArticle" sheetId="3" r:id="rId4"/>
     <sheet name="DivisionData" sheetId="4" r:id="rId5"/>
-    <sheet name="DependentTestData" sheetId="6" r:id="rId6"/>
+    <sheet name="AgentData" sheetId="7" r:id="rId6"/>
+    <sheet name="DependentTestData" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="60">
   <si>
     <t>TestId</t>
   </si>
@@ -169,6 +170,36 @@
   </si>
   <si>
     <t>AutoArticle Edit</t>
+  </si>
+  <si>
+    <t>AutoAgent</t>
+  </si>
+  <si>
+    <t>Agent_Email</t>
+  </si>
+  <si>
+    <t>kulwindersingh1@benicomp.com</t>
+  </si>
+  <si>
+    <t>BCP011_Test</t>
+  </si>
+  <si>
+    <t>Agency_Name</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>Agency1</t>
+  </si>
+  <si>
+    <t>Agency2</t>
+  </si>
+  <si>
+    <t>Agency3</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -227,7 +258,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -240,6 +271,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1039,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1080,10 +1112,117 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1095,7 +1234,7 @@
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>